<commit_message>
Adding support for user dashboard related testcases
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQABox2/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\LogixalQABox2\ALL_PAGES\END_TO_END\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23B773-CE74-4102-B47F-DCBCD2FB91E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TC02_Verify_MYACC" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="62">
   <si>
     <t>TestCase</t>
   </si>
@@ -89,9 +83,6 @@
     <t>MyaccountSection</t>
   </si>
   <si>
-    <t>ProfileSection</t>
-  </si>
-  <si>
     <t>PaymentInfo</t>
   </si>
   <si>
@@ -107,21 +98,9 @@
     <t>Quotes</t>
   </si>
   <si>
-    <t>Purchasing history</t>
-  </si>
-  <si>
-    <t>Quick order</t>
-  </si>
-  <si>
     <t>Accounts</t>
   </si>
   <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
     <t>Payment Info</t>
   </si>
   <si>
@@ -170,9 +149,6 @@
     <t>$Managed_Password</t>
   </si>
   <si>
-    <t>PurchasingHistory</t>
-  </si>
-  <si>
     <t>CSS</t>
   </si>
   <si>
@@ -185,9 +161,6 @@
     <t>MOUSEOVER</t>
   </si>
   <si>
-    <t>Sign out</t>
-  </si>
-  <si>
     <t>JSElement</t>
   </si>
   <si>
@@ -207,13 +180,34 @@
   </si>
   <si>
     <t>EnableCertificate_GoTOPage</t>
+  </si>
+  <si>
+    <t>DashboardSection</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>ProfileSettings</t>
+  </si>
+  <si>
+    <t>Profile Settings</t>
+  </si>
+  <si>
+    <t>Purchasinghistory</t>
+  </si>
+  <si>
+    <t>SignOut</t>
+  </si>
+  <si>
+    <t>Sign Out</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -223,6 +217,19 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -270,12 +277,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,11 +631,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD8"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -656,7 +666,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -670,22 +680,22 @@
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -694,22 +704,22 @@
     <row r="5" spans="1:5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -718,7 +728,7 @@
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -727,13 +737,13 @@
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -746,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -759,7 +769,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>14</v>
@@ -774,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>15</v>
@@ -789,14 +799,14 @@
         <v>16</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -811,46 +821,52 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>21</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
-        <v>17</v>
+      <c r="B17" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3"/>
@@ -858,13 +874,13 @@
         <v>11</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -873,13 +889,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -887,14 +903,14 @@
       <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
+      <c r="C20" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>24</v>
+        <v>44</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -902,14 +918,14 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>25</v>
+      <c r="C21" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -917,13 +933,13 @@
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -932,14 +948,14 @@
       <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
+      <c r="C23" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -947,14 +963,14 @@
       <c r="B24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
+      <c r="C24" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>28</v>
+        <v>44</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -962,14 +978,14 @@
       <c r="B25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>56</v>
+      <c r="C25" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -978,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -993,41 +1009,41 @@
         <v>11</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3"/>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>50</v>
+      <c r="C28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="E28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1049,7 +1065,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1057,7 +1073,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1065,7 +1081,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1094,103 +1110,103 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
+      <c r="A11" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>26</v>
+      <c r="A12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>56</v>
+      <c r="A16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="b">
         <v>1</v>
@@ -1198,15 +1214,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>1</v>
@@ -1214,7 +1230,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3" t="b">
         <v>1</v>
@@ -1222,7 +1238,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B24" s="3" t="b">
         <v>1</v>
@@ -1230,7 +1246,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="b">
         <v>1</v>
@@ -1238,23 +1254,23 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://192.168.15.18/storeus"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
@@ -1262,9 +1278,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1465,19 +1484,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1502,9 +1517,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>